<commit_message>
Updating paper + spreadsheet
</commit_message>
<xml_diff>
--- a/test_results.xlsx
+++ b/test_results.xlsx
@@ -4,10 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19260" windowHeight="12740" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20140" windowHeight="16260" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="results" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="46">
   <si>
     <t>F1</t>
   </si>
@@ -55,6 +58,108 @@
   </si>
   <si>
     <t>TEST DATA</t>
+  </si>
+  <si>
+    <t>Precision:</t>
+  </si>
+  <si>
+    <t>Recall:</t>
+  </si>
+  <si>
+    <t>F1:</t>
+  </si>
+  <si>
+    <t>All Singletons</t>
+  </si>
+  <si>
+    <t>+exactMatch</t>
+  </si>
+  <si>
+    <t>+headLowcaseMatch</t>
+  </si>
+  <si>
+    <t>+headExactMatch</t>
+  </si>
+  <si>
+    <t>Singleton</t>
+  </si>
+  <si>
+    <t>Singleton-exact</t>
+  </si>
+  <si>
+    <t>Singleton-exact-appositive</t>
+  </si>
+  <si>
+    <t>TRAINING</t>
+  </si>
+  <si>
+    <t>Singleton-exact-acronym</t>
+  </si>
+  <si>
+    <t>Singleton-exact-acronym-appositive</t>
+  </si>
+  <si>
+    <t>Singleton-exact-acronym-dropAfterHead</t>
+  </si>
+  <si>
+    <t>Singleton-exact-acronym-noStopWord</t>
+  </si>
+  <si>
+    <t>Singleton-exact-acronym-noStopWord-dropAfterHead</t>
+  </si>
+  <si>
+    <t>Singleton-exact-acronym-noStopWord-dropAfterHead-headExact-headLowcase</t>
+  </si>
+  <si>
+    <t>Singleton-exact-acronym-noStopWord-dropAfterHead-headExact</t>
+  </si>
+  <si>
+    <t>Singleton-exact-acronym-noStopWord-dropAfterHead-headExact-headLowcase-partialOverlap</t>
+  </si>
+  <si>
+    <t>Singleton-exact-acronym-noStopWord-dropAfterHead-headExact-headLowcase-headLemma</t>
+  </si>
+  <si>
+    <t>MY SHITTY ONE</t>
+  </si>
+  <si>
+    <t>JIE</t>
+  </si>
+  <si>
+    <t>Full</t>
+  </si>
+  <si>
+    <t>My Base + Jei Pronoun</t>
+  </si>
+  <si>
+    <t>No Person</t>
+  </si>
+  <si>
+    <t>All Singleton</t>
+  </si>
+  <si>
+    <t>OneCluster</t>
+  </si>
+  <si>
+    <t>B3</t>
+  </si>
+  <si>
+    <t>Baseline</t>
+  </si>
+  <si>
+    <t>BetterBaseline</t>
+  </si>
+  <si>
+    <t>RuleBased (test)</t>
+  </si>
+  <si>
+    <t>RuleBased (dev)</t>
+  </si>
+  <si>
+    <t>Classifier (dev)</t>
+  </si>
+  <si>
+    <t>Classifier (test)</t>
   </si>
 </sst>
 </file>
@@ -64,7 +169,14 @@
   <numFmts count="1">
     <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -140,33 +252,246 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="226">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -175,21 +500,240 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="13">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+  <cellStyles count="226">
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="71" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="73" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="87" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="89" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="91" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="93" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="105" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="107" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="109" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="111" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="113" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="115" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="117" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="119" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="121" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="123" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="125" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="127" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="129" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="131" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="133" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="135" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="137" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="139" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="141" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="143" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="145" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="147" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="149" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="151" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="153" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="155" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="157" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="159" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="161" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="163" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="165" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="167" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="169" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="171" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="173" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="175" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="177" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="179" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="181" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="183" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="185" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="187" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="189" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="191" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="193" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="195" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="197" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="199" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="201" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="203" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="205" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="207" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="209" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="211" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="213" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="215" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="217" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="219" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="221" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="223" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="225" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="32" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="34" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="36" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="38" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="40" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="50" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="52" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="54" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="62" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="64" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="66" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="68" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="70" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="72" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="74" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="76" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="78" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="80" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="82" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="84" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="86" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="88" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="90" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="92" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="94" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="96" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="98" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="100" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="102" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="104" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="106" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="108" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="110" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="112" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="114" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="116" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="118" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="120" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="122" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="124" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="126" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="128" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="130" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="132" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="134" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="136" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="138" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="140" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="142" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="144" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="146" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="148" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="150" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="152" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="154" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="156" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="158" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="160" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="162" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="164" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="166" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="168" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="170" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="172" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="174" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="176" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="178" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="180" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="182" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="184" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="186" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="188" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="190" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="192" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="194" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="196" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="198" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="200" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="202" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="204" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="206" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="208" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="210" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="212" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="214" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="216" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="218" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="220" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="222" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="224" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -520,7 +1064,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
@@ -720,4 +1264,1233 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B4:O41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="4" spans="2:15">
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15">
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>0.96941099902375505</v>
+      </c>
+      <c r="G5">
+        <v>0.96393546346092995</v>
+      </c>
+      <c r="H5">
+        <v>0.96364211191906401</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15">
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0.46972563859980998</v>
+      </c>
+      <c r="G6">
+        <v>0.48044780826237699</v>
+      </c>
+      <c r="H6">
+        <v>0.480605487228003</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15">
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0.63281996813595298</v>
+      </c>
+      <c r="G7">
+        <v>0.64127117752288698</v>
+      </c>
+      <c r="H7">
+        <v>0.64134665965281401</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15">
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>0.95368586020409596</v>
+      </c>
+      <c r="G9">
+        <v>0.94960074891637203</v>
+      </c>
+      <c r="H9">
+        <v>0.94939446883386003</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15">
+      <c r="B10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10">
+        <v>0.27320650928260298</v>
+      </c>
+      <c r="F10">
+        <v>0.53212752326287105</v>
+      </c>
+      <c r="G10">
+        <v>0.54292146106443495</v>
+      </c>
+      <c r="H10">
+        <v>0.54303606111027503</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15">
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11">
+        <v>0.429162916291629</v>
+      </c>
+      <c r="F11">
+        <v>0.68310394886479897</v>
+      </c>
+      <c r="G11">
+        <v>0.69085554986305797</v>
+      </c>
+      <c r="H11">
+        <v>0.69089370989310905</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15">
+      <c r="D13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15">
+      <c r="D14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" t="s">
+        <v>23</v>
+      </c>
+      <c r="H14" t="s">
+        <v>24</v>
+      </c>
+      <c r="I14" t="s">
+        <v>25</v>
+      </c>
+      <c r="J14" t="s">
+        <v>26</v>
+      </c>
+      <c r="K14" t="s">
+        <v>27</v>
+      </c>
+      <c r="L14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M14" t="s">
+        <v>28</v>
+      </c>
+      <c r="N14" t="s">
+        <v>30</v>
+      </c>
+      <c r="O14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15">
+      <c r="C15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15">
+        <v>1.08235054900366</v>
+      </c>
+      <c r="F15">
+        <v>1.08056006493506</v>
+      </c>
+      <c r="G15">
+        <v>1.0734808289118001</v>
+      </c>
+      <c r="H15">
+        <v>1.0717354381057</v>
+      </c>
+      <c r="I15">
+        <v>1.0314082278481</v>
+      </c>
+      <c r="J15">
+        <v>1.0410229088971701</v>
+      </c>
+      <c r="K15">
+        <v>1.02302221570496</v>
+      </c>
+      <c r="L15">
+        <v>0.97546674895849395</v>
+      </c>
+      <c r="M15">
+        <v>0.97190504807692302</v>
+      </c>
+      <c r="N15">
+        <v>0.96469829937032003</v>
+      </c>
+      <c r="O15">
+        <v>0.96075160673109905</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15">
+      <c r="E16">
+        <v>0.24771965748324601</v>
+      </c>
+      <c r="F16">
+        <v>0.24781273268801099</v>
+      </c>
+      <c r="G16">
+        <v>0.24951135517498099</v>
+      </c>
+      <c r="H16">
+        <v>0.249604430379746</v>
+      </c>
+      <c r="I16">
+        <v>0.30335536113179401</v>
+      </c>
+      <c r="J16">
+        <v>0.30810469883317498</v>
+      </c>
+      <c r="K16">
+        <v>0.32466958302308202</v>
+      </c>
+      <c r="L16">
+        <v>0.44131608339538297</v>
+      </c>
+      <c r="M16">
+        <v>0.45157762472077401</v>
+      </c>
+      <c r="N16">
+        <v>0.45274106478034198</v>
+      </c>
+      <c r="O16">
+        <v>0.45567293373045398</v>
+      </c>
+    </row>
+    <row r="17" spans="3:15">
+      <c r="E17">
+        <v>0.40316594713322701</v>
+      </c>
+      <c r="F17">
+        <v>0.40316474863718899</v>
+      </c>
+      <c r="G17">
+        <v>0.404908902105163</v>
+      </c>
+      <c r="H17">
+        <v>0.40490704916485698</v>
+      </c>
+      <c r="I17">
+        <v>0.468821921749137</v>
+      </c>
+      <c r="J17">
+        <v>0.47548363547876799</v>
+      </c>
+      <c r="K17">
+        <v>0.49290823986575899</v>
+      </c>
+      <c r="L17">
+        <v>0.60769957865393498</v>
+      </c>
+      <c r="M17">
+        <v>0.61664336553126498</v>
+      </c>
+      <c r="N17">
+        <v>0.61626415393142697</v>
+      </c>
+      <c r="O17">
+        <v>0.61816000883852296</v>
+      </c>
+    </row>
+    <row r="19" spans="3:15">
+      <c r="E19">
+        <v>0.99214404439183901</v>
+      </c>
+      <c r="F19">
+        <v>0.99179349140289796</v>
+      </c>
+      <c r="G19">
+        <v>0.99042417212261702</v>
+      </c>
+      <c r="H19">
+        <v>0.99007361913367697</v>
+      </c>
+      <c r="I19">
+        <v>0.98008250064411295</v>
+      </c>
+      <c r="J19">
+        <v>0.98711158770177698</v>
+      </c>
+      <c r="K19">
+        <v>0.97720263502094995</v>
+      </c>
+      <c r="L19">
+        <v>0.95088591880193196</v>
+      </c>
+      <c r="M19">
+        <v>0.94845224686930996</v>
+      </c>
+      <c r="N19">
+        <v>0.94423441105585604</v>
+      </c>
+      <c r="O19">
+        <v>0.942240957000818</v>
+      </c>
+    </row>
+    <row r="20" spans="3:15">
+      <c r="E20">
+        <v>0.38626337271792699</v>
+      </c>
+      <c r="F20">
+        <v>0.38632049157554998</v>
+      </c>
+      <c r="G20">
+        <v>0.38732891371479999</v>
+      </c>
+      <c r="H20">
+        <v>0.38738603257242299</v>
+      </c>
+      <c r="I20">
+        <v>0.42384260204927998</v>
+      </c>
+      <c r="J20">
+        <v>0.42099034567840798</v>
+      </c>
+      <c r="K20">
+        <v>0.43841777492462802</v>
+      </c>
+      <c r="L20">
+        <v>0.51320485720506603</v>
+      </c>
+      <c r="M20">
+        <v>0.52161834946556096</v>
+      </c>
+      <c r="N20">
+        <v>0.52245474259996605</v>
+      </c>
+      <c r="O20">
+        <v>0.52458035689208005</v>
+      </c>
+    </row>
+    <row r="21" spans="3:15">
+      <c r="E21">
+        <v>0.556045912190966</v>
+      </c>
+      <c r="F21">
+        <v>0.55605001309415003</v>
+      </c>
+      <c r="G21">
+        <v>0.55687760404755504</v>
+      </c>
+      <c r="H21">
+        <v>0.55688119909104805</v>
+      </c>
+      <c r="I21">
+        <v>0.59177048191393</v>
+      </c>
+      <c r="J21">
+        <v>0.59024767835118397</v>
+      </c>
+      <c r="K21">
+        <v>0.60527949708331596</v>
+      </c>
+      <c r="L21">
+        <v>0.66662433801812404</v>
+      </c>
+      <c r="M21">
+        <v>0.673069846839079</v>
+      </c>
+      <c r="N21">
+        <v>0.67269843095598703</v>
+      </c>
+      <c r="O21">
+        <v>0.67394861639965897</v>
+      </c>
+    </row>
+    <row r="23" spans="3:15">
+      <c r="C23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="3:15">
+      <c r="N25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="3:15">
+      <c r="J26" t="s">
+        <v>3</v>
+      </c>
+      <c r="K26" t="s">
+        <v>12</v>
+      </c>
+      <c r="M26">
+        <v>0.79132223233002397</v>
+      </c>
+      <c r="N26">
+        <v>0.85823754789272</v>
+      </c>
+    </row>
+    <row r="27" spans="3:15">
+      <c r="J27" t="s">
+        <v>3</v>
+      </c>
+      <c r="K27" t="s">
+        <v>13</v>
+      </c>
+      <c r="M27">
+        <v>0.46553890543559101</v>
+      </c>
+      <c r="N27">
+        <v>0.620253164556962</v>
+      </c>
+    </row>
+    <row r="28" spans="3:15">
+      <c r="J28" t="s">
+        <v>3</v>
+      </c>
+      <c r="K28" t="s">
+        <v>14</v>
+      </c>
+      <c r="M28">
+        <v>0.58620841207752805</v>
+      </c>
+      <c r="N28">
+        <v>0.72009184845005703</v>
+      </c>
+    </row>
+    <row r="29" spans="3:15">
+      <c r="K29" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="3:15">
+      <c r="J30" t="s">
+        <v>4</v>
+      </c>
+      <c r="K30" t="s">
+        <v>12</v>
+      </c>
+      <c r="M30">
+        <v>0.84609081317427404</v>
+      </c>
+      <c r="N30">
+        <v>0.84826501671828203</v>
+      </c>
+    </row>
+    <row r="31" spans="3:15">
+      <c r="E31" t="s">
+        <v>36</v>
+      </c>
+      <c r="J31" t="s">
+        <v>4</v>
+      </c>
+      <c r="K31" t="s">
+        <v>13</v>
+      </c>
+      <c r="M31">
+        <v>0.47224008921875099</v>
+      </c>
+      <c r="N31">
+        <v>0.58406437091473995</v>
+      </c>
+    </row>
+    <row r="32" spans="3:15">
+      <c r="E32">
+        <v>0.84829147797447502</v>
+      </c>
+      <c r="F32">
+        <v>0.84829147797447502</v>
+      </c>
+      <c r="J32" t="s">
+        <v>4</v>
+      </c>
+      <c r="K32" t="s">
+        <v>14</v>
+      </c>
+      <c r="M32">
+        <v>0.60615737729474395</v>
+      </c>
+      <c r="N32">
+        <v>0.69179809844896101</v>
+      </c>
+    </row>
+    <row r="33" spans="5:11">
+      <c r="E33">
+        <v>0.64979501734468603</v>
+      </c>
+      <c r="F33">
+        <v>0.64979501734468603</v>
+      </c>
+    </row>
+    <row r="34" spans="5:11">
+      <c r="E34">
+        <v>0.73589285714285702</v>
+      </c>
+      <c r="F34">
+        <v>0.73589285714285702</v>
+      </c>
+      <c r="K34" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" spans="5:11">
+      <c r="K35">
+        <v>0.85867532723157103</v>
+      </c>
+    </row>
+    <row r="36" spans="5:11">
+      <c r="E36">
+        <v>0.84239280304725905</v>
+      </c>
+      <c r="F36">
+        <v>0.84239280304725905</v>
+      </c>
+      <c r="K36">
+        <v>0.60906087118391605</v>
+      </c>
+    </row>
+    <row r="37" spans="5:11">
+      <c r="E37">
+        <v>0.625891973975222</v>
+      </c>
+      <c r="F37">
+        <v>0.625891973975222</v>
+      </c>
+      <c r="K37">
+        <v>0.71264242638750797</v>
+      </c>
+    </row>
+    <row r="38" spans="5:11">
+      <c r="E38">
+        <v>0.71818069983803501</v>
+      </c>
+      <c r="F38">
+        <v>0.71818069983803501</v>
+      </c>
+    </row>
+    <row r="39" spans="5:11">
+      <c r="K39">
+        <v>0.84859900609230698</v>
+      </c>
+    </row>
+    <row r="40" spans="5:11">
+      <c r="K40">
+        <v>0.57495010126433399</v>
+      </c>
+    </row>
+    <row r="41" spans="5:11">
+      <c r="K41">
+        <v>0.68547278343148998</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:O19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="2:13">
+      <c r="D1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="2:13">
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="8">
+        <v>1</v>
+      </c>
+      <c r="E2" s="8">
+        <v>0.76938637896156403</v>
+      </c>
+    </row>
+    <row r="3" spans="2:13">
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="8">
+        <v>0</v>
+      </c>
+      <c r="E3" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13">
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="8">
+        <v>0</v>
+      </c>
+      <c r="E4" s="8">
+        <v>0.86966463414634099</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13">
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="8">
+        <v>1</v>
+      </c>
+      <c r="E5" s="8">
+        <v>0.16460551033160301</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13">
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="8">
+        <v>0.246616044899306</v>
+      </c>
+      <c r="E6" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13">
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="8">
+        <v>0.39565677966101598</v>
+      </c>
+      <c r="E7" s="8">
+        <v>0.28268028765334402</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13">
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="11" spans="2:13">
+      <c r="C11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13">
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13">
+      <c r="B13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="9">
+        <v>1</v>
+      </c>
+      <c r="D13" s="9">
+        <v>0</v>
+      </c>
+      <c r="E13" s="9">
+        <v>0</v>
+      </c>
+      <c r="F13" s="9">
+        <v>1</v>
+      </c>
+      <c r="G13" s="9">
+        <v>0.246616044899306</v>
+      </c>
+      <c r="H13" s="9">
+        <v>0.39565677966101598</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13">
+      <c r="B14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="9">
+        <v>0.76938637896156403</v>
+      </c>
+      <c r="D14" s="9">
+        <v>1</v>
+      </c>
+      <c r="E14" s="9">
+        <v>0.86966463414634099</v>
+      </c>
+      <c r="F14" s="9">
+        <v>0.16460551033160301</v>
+      </c>
+      <c r="G14" s="9">
+        <v>1</v>
+      </c>
+      <c r="H14" s="9">
+        <v>0.28268028765334402</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13">
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+    </row>
+    <row r="16" spans="2:13">
+      <c r="C16" t="s">
+        <v>3</v>
+      </c>
+      <c r="F16" t="s">
+        <v>39</v>
+      </c>
+      <c r="J16" t="s">
+        <v>3</v>
+      </c>
+      <c r="M16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15">
+      <c r="C17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" t="s">
+        <v>13</v>
+      </c>
+      <c r="H17" t="s">
+        <v>14</v>
+      </c>
+      <c r="J17" t="s">
+        <v>12</v>
+      </c>
+      <c r="K17" t="s">
+        <v>13</v>
+      </c>
+      <c r="L17" t="s">
+        <v>14</v>
+      </c>
+      <c r="M17" t="s">
+        <v>12</v>
+      </c>
+      <c r="N17" t="s">
+        <v>13</v>
+      </c>
+      <c r="O17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15">
+      <c r="B18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="9">
+        <v>0.805614035087719</v>
+      </c>
+      <c r="D18" s="9">
+        <v>0.503067484662576</v>
+      </c>
+      <c r="E18" s="9">
+        <v>0.61936876180199596</v>
+      </c>
+      <c r="F18" s="9">
+        <v>0.86282320567563198</v>
+      </c>
+      <c r="G18" s="9">
+        <v>0.44896962207082203</v>
+      </c>
+      <c r="H18" s="9">
+        <v>0.59061370114610401</v>
+      </c>
+      <c r="I18" t="s">
+        <v>40</v>
+      </c>
+      <c r="J18" s="9">
+        <v>0.80754352030947696</v>
+      </c>
+      <c r="K18" s="9">
+        <v>0.39498580889309298</v>
+      </c>
+      <c r="L18" s="9">
+        <v>0.53049555273189297</v>
+      </c>
+      <c r="M18" s="9">
+        <v>0.91307382645597202</v>
+      </c>
+      <c r="N18" s="9">
+        <v>0.43566861503042797</v>
+      </c>
+      <c r="O18" s="9">
+        <v>0.58987927888471903</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15">
+      <c r="B19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="9">
+        <v>0.83343428225317895</v>
+      </c>
+      <c r="D19" s="9">
+        <v>0.60297984224364498</v>
+      </c>
+      <c r="E19" s="9">
+        <v>0.69972031528095502</v>
+      </c>
+      <c r="F19" s="9">
+        <v>0.83407636651281403</v>
+      </c>
+      <c r="G19" s="9">
+        <v>0.51412623104877697</v>
+      </c>
+      <c r="H19" s="9">
+        <v>0.63613664518622404</v>
+      </c>
+      <c r="I19" t="s">
+        <v>41</v>
+      </c>
+      <c r="J19" s="9">
+        <v>0.85299539170506899</v>
+      </c>
+      <c r="K19" s="9">
+        <v>0.58372753074739803</v>
+      </c>
+      <c r="L19" s="9">
+        <v>0.69312862759782801</v>
+      </c>
+      <c r="M19" s="9">
+        <v>0.87325378978402601</v>
+      </c>
+      <c r="N19" s="9">
+        <v>0.56491019127683695</v>
+      </c>
+      <c r="O19" s="9">
+        <v>0.68602742373818404</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:L29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N27" sqref="N27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="3" spans="2:10">
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3">
+        <v>0.84133280444268099</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10">
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4">
+        <v>0.66887417218542999</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10">
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5">
+        <v>0.74525650035137003</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10">
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>0.82287732426736704</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10">
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7">
+        <v>0.64159001322797804</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10">
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8">
+        <v>0.72101283496653101</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10">
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10">
+      <c r="D13" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="10">
+        <v>0.79845360824742195</v>
+      </c>
+      <c r="F13" s="10">
+        <v>0.67879053461875505</v>
+      </c>
+      <c r="G13" s="10">
+        <v>0.73377546186641396</v>
+      </c>
+      <c r="H13" s="10">
+        <v>0.73088519424443399</v>
+      </c>
+      <c r="I13" s="10">
+        <v>0.58713468772000299</v>
+      </c>
+      <c r="J13" s="10">
+        <v>0.65117083005195298</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10">
+      <c r="D14" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" s="10">
+        <v>0.84133280444268099</v>
+      </c>
+      <c r="F14" s="10">
+        <v>0.66887417218542999</v>
+      </c>
+      <c r="G14" s="10">
+        <v>0.74525650035137003</v>
+      </c>
+      <c r="H14" s="10">
+        <v>0.82287732426736704</v>
+      </c>
+      <c r="I14" s="10">
+        <v>0.64159001322797804</v>
+      </c>
+      <c r="J14" s="10">
+        <v>0.72101283496653101</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10">
+      <c r="D15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" s="10">
+        <v>0.81688654353561996</v>
+      </c>
+      <c r="F15" s="10">
+        <v>0.67835232252410105</v>
+      </c>
+      <c r="G15" s="10">
+        <v>0.74120181948767005</v>
+      </c>
+      <c r="H15" s="10">
+        <v>0.80817378131740703</v>
+      </c>
+      <c r="I15" s="10">
+        <v>0.57921612930912203</v>
+      </c>
+      <c r="J15" s="10">
+        <v>0.67480278736118704</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10">
+      <c r="D16" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" s="10">
+        <v>0.81759352881698599</v>
+      </c>
+      <c r="F16" s="10">
+        <v>0.63749605802585896</v>
+      </c>
+      <c r="G16" s="10">
+        <v>0.716399397536989</v>
+      </c>
+      <c r="H16" s="10">
+        <v>0.84367450912068898</v>
+      </c>
+      <c r="I16" s="10">
+        <v>0.59923951478536297</v>
+      </c>
+      <c r="J16" s="10">
+        <v>0.70075291404219997</v>
+      </c>
+    </row>
+    <row r="22" spans="6:12">
+      <c r="F22" t="s">
+        <v>3</v>
+      </c>
+      <c r="G22" t="s">
+        <v>12</v>
+      </c>
+      <c r="H22">
+        <v>0.81688654353561996</v>
+      </c>
+    </row>
+    <row r="23" spans="6:12">
+      <c r="F23" t="s">
+        <v>3</v>
+      </c>
+      <c r="G23" t="s">
+        <v>13</v>
+      </c>
+      <c r="H23">
+        <v>0.67835232252410105</v>
+      </c>
+      <c r="J23" t="s">
+        <v>3</v>
+      </c>
+      <c r="K23" t="s">
+        <v>12</v>
+      </c>
+      <c r="L23">
+        <v>0.81759352881698599</v>
+      </c>
+    </row>
+    <row r="24" spans="6:12">
+      <c r="F24" t="s">
+        <v>3</v>
+      </c>
+      <c r="G24" t="s">
+        <v>14</v>
+      </c>
+      <c r="H24">
+        <v>0.74120181948767005</v>
+      </c>
+      <c r="J24" t="s">
+        <v>3</v>
+      </c>
+      <c r="K24" t="s">
+        <v>13</v>
+      </c>
+      <c r="L24">
+        <v>0.63749605802585896</v>
+      </c>
+    </row>
+    <row r="25" spans="6:12">
+      <c r="G25" t="s">
+        <v>4</v>
+      </c>
+      <c r="H25">
+        <v>0.80817378131740703</v>
+      </c>
+      <c r="J25" t="s">
+        <v>3</v>
+      </c>
+      <c r="K25" t="s">
+        <v>14</v>
+      </c>
+      <c r="L25">
+        <v>0.716399397536989</v>
+      </c>
+    </row>
+    <row r="26" spans="6:12">
+      <c r="F26" t="s">
+        <v>4</v>
+      </c>
+      <c r="G26" t="s">
+        <v>12</v>
+      </c>
+      <c r="H26">
+        <v>0.57921612930912203</v>
+      </c>
+      <c r="K26" t="s">
+        <v>4</v>
+      </c>
+      <c r="L26">
+        <v>0.84367450912068898</v>
+      </c>
+    </row>
+    <row r="27" spans="6:12">
+      <c r="F27" t="s">
+        <v>4</v>
+      </c>
+      <c r="G27" t="s">
+        <v>13</v>
+      </c>
+      <c r="H27">
+        <v>0.67480278736118704</v>
+      </c>
+      <c r="J27" t="s">
+        <v>4</v>
+      </c>
+      <c r="K27" t="s">
+        <v>12</v>
+      </c>
+      <c r="L27">
+        <v>0.59923951478536297</v>
+      </c>
+    </row>
+    <row r="28" spans="6:12">
+      <c r="F28" t="s">
+        <v>4</v>
+      </c>
+      <c r="G28" t="s">
+        <v>14</v>
+      </c>
+      <c r="J28" t="s">
+        <v>4</v>
+      </c>
+      <c r="K28" t="s">
+        <v>13</v>
+      </c>
+      <c r="L28">
+        <v>0.70075291404219997</v>
+      </c>
+    </row>
+    <row r="29" spans="6:12">
+      <c r="J29" t="s">
+        <v>4</v>
+      </c>
+      <c r="K29" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Final base paper updates
</commit_message>
<xml_diff>
--- a/test_results.xlsx
+++ b/test_results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20140" windowHeight="16260" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20140" windowHeight="16260" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="results" sheetId="1" r:id="rId1"/>
@@ -167,7 +167,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.00000"/>
+    <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -252,9 +252,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="226">
+  <cellStyleXfs count="228">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -483,12 +485,6 @@
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -497,7 +493,7 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -506,8 +502,14 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="226">
+  <cellStyles count="228">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -620,6 +622,7 @@
     <cellStyle name="Followed Hyperlink" xfId="221" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="223" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="225" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="227" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -732,6 +735,7 @@
     <cellStyle name="Hyperlink" xfId="220" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="222" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="224" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="226" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -1071,44 +1075,44 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="4" spans="2:8">
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
     </row>
     <row r="5" spans="2:8">
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3" t="s">
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
     </row>
     <row r="6" spans="2:8">
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="H6" s="2" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1116,45 +1120,45 @@
       <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="4">
         <v>0.80615566735720601</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="4">
         <v>0.42951750236518399</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="4">
         <v>0.56043616911840299</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="4">
         <v>0.899118665653039</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="4">
         <v>0.455361741315576</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="4">
         <v>0.60454804533852802</v>
       </c>
     </row>
     <row r="8" spans="2:8">
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="4">
         <v>0.80615566735720601</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="4">
         <v>0.42951750236518399</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="4">
         <v>0.56043616911840299</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="4">
         <v>0.899118665653039</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="4">
         <v>0.455361741315576</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H8" s="4">
         <v>0.60454804533852802</v>
       </c>
     </row>
@@ -1162,22 +1166,22 @@
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="4">
         <v>0.83590462833099499</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="4">
         <v>0.469883317565436</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="4">
         <v>0.60159483193701402</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="4">
         <v>0.89208920963779403</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="4">
         <v>0.48262699229795097</v>
       </c>
-      <c r="H9" s="6">
+      <c r="H9" s="4">
         <v>0.62637849397961598</v>
       </c>
     </row>
@@ -1185,22 +1189,22 @@
       <c r="B10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="4">
         <v>0.83590462833099499</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="4">
         <v>0.469883317565436</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="4">
         <v>0.60159483193701402</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="4">
         <v>0.89208920963779403</v>
       </c>
-      <c r="G10" s="6">
+      <c r="G10" s="4">
         <v>0.48262699229795097</v>
       </c>
-      <c r="H10" s="6">
+      <c r="H10" s="4">
         <v>0.62637849397961598</v>
       </c>
     </row>
@@ -1208,22 +1212,22 @@
       <c r="B11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="4">
         <v>0.79325666492420199</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="4">
         <v>0.47855566067486599</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="4">
         <v>0.59697088906372897</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11" s="4">
         <v>0.84826600521607498</v>
       </c>
-      <c r="G11" s="6">
+      <c r="G11" s="4">
         <v>0.486144057164419</v>
       </c>
-      <c r="H11" s="6">
+      <c r="H11" s="4">
         <v>0.61807009547685998</v>
       </c>
     </row>
@@ -1231,22 +1235,22 @@
       <c r="B12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="4">
         <v>0.85029686174724295</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="4">
         <v>0.63229265216020103</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="4">
         <v>0.72526677518538596</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="4">
         <v>0.84536935277434599</v>
       </c>
-      <c r="G12" s="6">
+      <c r="G12" s="4">
         <v>0.59688137520594498</v>
       </c>
-      <c r="H12" s="6">
+      <c r="H12" s="4">
         <v>0.69971914321378204</v>
       </c>
     </row>
@@ -1270,8 +1274,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:O41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1280,13 +1284,13 @@
       <c r="D4" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="5" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1669,6 +1673,13 @@
     <row r="23" spans="3:15">
       <c r="C23" t="s">
         <v>33</v>
+      </c>
+      <c r="G23" s="8"/>
+    </row>
+    <row r="24" spans="3:15">
+      <c r="G24" s="8">
+        <f>G21-E21</f>
+        <v>8.3169185658904521E-4</v>
       </c>
     </row>
     <row r="25" spans="3:15">
@@ -1879,10 +1890,10 @@
       <c r="C2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="8">
+      <c r="D2" s="6">
         <v>1</v>
       </c>
-      <c r="E2" s="8">
+      <c r="E2" s="6">
         <v>0.76938637896156403</v>
       </c>
     </row>
@@ -1890,10 +1901,10 @@
       <c r="C3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="6">
         <v>0</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="6">
         <v>1</v>
       </c>
     </row>
@@ -1901,10 +1912,10 @@
       <c r="C4" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="6">
         <v>0</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="6">
         <v>0.86966463414634099</v>
       </c>
     </row>
@@ -1915,10 +1926,10 @@
       <c r="C5" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="6">
         <v>1</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="6">
         <v>0.16460551033160301</v>
       </c>
     </row>
@@ -1926,10 +1937,10 @@
       <c r="C6" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="6">
         <v>0.246616044899306</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="6">
         <v>1</v>
       </c>
     </row>
@@ -1937,10 +1948,10 @@
       <c r="C7" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="6">
         <v>0.39565677966101598</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="6">
         <v>0.28268028765334402</v>
       </c>
     </row>
@@ -1980,22 +1991,22 @@
       <c r="B13" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="7">
         <v>1</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D13" s="7">
         <v>0</v>
       </c>
-      <c r="E13" s="9">
+      <c r="E13" s="7">
         <v>0</v>
       </c>
-      <c r="F13" s="9">
+      <c r="F13" s="7">
         <v>1</v>
       </c>
-      <c r="G13" s="9">
+      <c r="G13" s="7">
         <v>0.246616044899306</v>
       </c>
-      <c r="H13" s="9">
+      <c r="H13" s="7">
         <v>0.39565677966101598</v>
       </c>
     </row>
@@ -2003,32 +2014,32 @@
       <c r="B14" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="9">
+      <c r="C14" s="7">
         <v>0.76938637896156403</v>
       </c>
-      <c r="D14" s="9">
+      <c r="D14" s="7">
         <v>1</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E14" s="7">
         <v>0.86966463414634099</v>
       </c>
-      <c r="F14" s="9">
+      <c r="F14" s="7">
         <v>0.16460551033160301</v>
       </c>
-      <c r="G14" s="9">
+      <c r="G14" s="7">
         <v>1</v>
       </c>
-      <c r="H14" s="9">
+      <c r="H14" s="7">
         <v>0.28268028765334402</v>
       </c>
     </row>
     <row r="15" spans="2:13">
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
     </row>
     <row r="16" spans="2:13">
       <c r="C16" t="s">
@@ -2086,43 +2097,43 @@
       <c r="B18" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="9">
+      <c r="C18" s="7">
         <v>0.805614035087719</v>
       </c>
-      <c r="D18" s="9">
+      <c r="D18" s="7">
         <v>0.503067484662576</v>
       </c>
-      <c r="E18" s="9">
+      <c r="E18" s="7">
         <v>0.61936876180199596</v>
       </c>
-      <c r="F18" s="9">
+      <c r="F18" s="7">
         <v>0.86282320567563198</v>
       </c>
-      <c r="G18" s="9">
+      <c r="G18" s="7">
         <v>0.44896962207082203</v>
       </c>
-      <c r="H18" s="9">
+      <c r="H18" s="7">
         <v>0.59061370114610401</v>
       </c>
       <c r="I18" t="s">
         <v>40</v>
       </c>
-      <c r="J18" s="9">
+      <c r="J18" s="7">
         <v>0.80754352030947696</v>
       </c>
-      <c r="K18" s="9">
+      <c r="K18" s="7">
         <v>0.39498580889309298</v>
       </c>
-      <c r="L18" s="9">
+      <c r="L18" s="7">
         <v>0.53049555273189297</v>
       </c>
-      <c r="M18" s="9">
+      <c r="M18" s="7">
         <v>0.91307382645597202</v>
       </c>
-      <c r="N18" s="9">
+      <c r="N18" s="7">
         <v>0.43566861503042797</v>
       </c>
-      <c r="O18" s="9">
+      <c r="O18" s="7">
         <v>0.58987927888471903</v>
       </c>
     </row>
@@ -2130,43 +2141,43 @@
       <c r="B19" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="9">
+      <c r="C19" s="7">
         <v>0.83343428225317895</v>
       </c>
-      <c r="D19" s="9">
+      <c r="D19" s="7">
         <v>0.60297984224364498</v>
       </c>
-      <c r="E19" s="9">
+      <c r="E19" s="7">
         <v>0.69972031528095502</v>
       </c>
-      <c r="F19" s="9">
+      <c r="F19" s="7">
         <v>0.83407636651281403</v>
       </c>
-      <c r="G19" s="9">
+      <c r="G19" s="7">
         <v>0.51412623104877697</v>
       </c>
-      <c r="H19" s="9">
+      <c r="H19" s="7">
         <v>0.63613664518622404</v>
       </c>
       <c r="I19" t="s">
         <v>41</v>
       </c>
-      <c r="J19" s="9">
+      <c r="J19" s="7">
         <v>0.85299539170506899</v>
       </c>
-      <c r="K19" s="9">
+      <c r="K19" s="7">
         <v>0.58372753074739803</v>
       </c>
-      <c r="L19" s="9">
+      <c r="L19" s="7">
         <v>0.69312862759782801</v>
       </c>
-      <c r="M19" s="9">
+      <c r="M19" s="7">
         <v>0.87325378978402601</v>
       </c>
-      <c r="N19" s="9">
+      <c r="N19" s="7">
         <v>0.56491019127683695</v>
       </c>
-      <c r="O19" s="9">
+      <c r="O19" s="7">
         <v>0.68602742373818404</v>
       </c>
     </row>
@@ -2185,8 +2196,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:L29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N27" sqref="N27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2266,22 +2277,22 @@
       <c r="D13" t="s">
         <v>43</v>
       </c>
-      <c r="E13" s="10">
+      <c r="E13" s="8">
         <v>0.79845360824742195</v>
       </c>
-      <c r="F13" s="10">
+      <c r="F13" s="8">
         <v>0.67879053461875505</v>
       </c>
-      <c r="G13" s="10">
+      <c r="G13" s="8">
         <v>0.73377546186641396</v>
       </c>
-      <c r="H13" s="10">
+      <c r="H13" s="8">
         <v>0.73088519424443399</v>
       </c>
-      <c r="I13" s="10">
+      <c r="I13" s="8">
         <v>0.58713468772000299</v>
       </c>
-      <c r="J13" s="10">
+      <c r="J13" s="8">
         <v>0.65117083005195298</v>
       </c>
     </row>
@@ -2289,22 +2300,22 @@
       <c r="D14" t="s">
         <v>42</v>
       </c>
-      <c r="E14" s="10">
+      <c r="E14" s="8">
         <v>0.84133280444268099</v>
       </c>
-      <c r="F14" s="10">
+      <c r="F14" s="8">
         <v>0.66887417218542999</v>
       </c>
-      <c r="G14" s="10">
+      <c r="G14" s="8">
         <v>0.74525650035137003</v>
       </c>
-      <c r="H14" s="10">
+      <c r="H14" s="8">
         <v>0.82287732426736704</v>
       </c>
-      <c r="I14" s="10">
+      <c r="I14" s="8">
         <v>0.64159001322797804</v>
       </c>
-      <c r="J14" s="10">
+      <c r="J14" s="8">
         <v>0.72101283496653101</v>
       </c>
     </row>
@@ -2312,22 +2323,22 @@
       <c r="D15" t="s">
         <v>44</v>
       </c>
-      <c r="E15" s="10">
+      <c r="E15" s="8">
         <v>0.81688654353561996</v>
       </c>
-      <c r="F15" s="10">
+      <c r="F15" s="8">
         <v>0.67835232252410105</v>
       </c>
-      <c r="G15" s="10">
+      <c r="G15" s="8">
         <v>0.74120181948767005</v>
       </c>
-      <c r="H15" s="10">
+      <c r="H15" s="8">
         <v>0.80817378131740703</v>
       </c>
-      <c r="I15" s="10">
+      <c r="I15" s="8">
         <v>0.57921612930912203</v>
       </c>
-      <c r="J15" s="10">
+      <c r="J15" s="8">
         <v>0.67480278736118704</v>
       </c>
     </row>
@@ -2335,22 +2346,22 @@
       <c r="D16" t="s">
         <v>45</v>
       </c>
-      <c r="E16" s="10">
+      <c r="E16" s="8">
         <v>0.81759352881698599</v>
       </c>
-      <c r="F16" s="10">
+      <c r="F16" s="8">
         <v>0.63749605802585896</v>
       </c>
-      <c r="G16" s="10">
+      <c r="G16" s="8">
         <v>0.716399397536989</v>
       </c>
-      <c r="H16" s="10">
+      <c r="H16" s="8">
         <v>0.84367450912068898</v>
       </c>
-      <c r="I16" s="10">
+      <c r="I16" s="8">
         <v>0.59923951478536297</v>
       </c>
-      <c r="J16" s="10">
+      <c r="J16" s="8">
         <v>0.70075291404219997</v>
       </c>
     </row>

</xml_diff>